<commit_message>
[*Full working*] Add toolkit_comparison.xlsx + Fix commented stuff
</commit_message>
<xml_diff>
--- a/translation/tmp/toolkit_comparison.xlsx
+++ b/translation/tmp/toolkit_comparison.xlsx
@@ -12,12 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="89">
   <si>
     <t>Fairseq</t>
   </si>
   <si>
     <t xml:space="preserve">↔ </t>
+  </si>
+  <si>
+    <t>Fairseq (layers1)</t>
   </si>
   <si>
     <t>Dataset</t>
@@ -233,6 +236,9 @@
     <t>bleu 36.7</t>
   </si>
   <si>
+    <t>bleu 36.96</t>
+  </si>
+  <si>
     <t>BLEU-b5 (sacrebleu)</t>
   </si>
   <si>
@@ -240,6 +246,21 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Fairseq (gpu22)</t>
+  </si>
+  <si>
+    <t>3087MiB+3087MiB</t>
+  </si>
+  <si>
+    <t>3645MiB</t>
+  </si>
+  <si>
+    <t>bleu 36.6</t>
+  </si>
+  <si>
+    <t>bleu 36.64</t>
   </si>
   <si>
     <t>Bentrevett</t>
@@ -689,6 +710,7 @@
     <col customWidth="1" min="24" max="24" width="7.57"/>
     <col customWidth="1" min="25" max="25" width="21.14"/>
     <col customWidth="1" min="29" max="29" width="22.86"/>
+    <col customWidth="1" min="31" max="31" width="22.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -728,899 +750,986 @@
       </c>
       <c r="Z1" s="8"/>
       <c r="AB1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>2</v>
-      </c>
       <c r="E2" s="10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>2</v>
-      </c>
       <c r="K2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>2</v>
-      </c>
       <c r="N2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="9" t="s">
-        <v>2</v>
-      </c>
       <c r="Q2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="9" t="s">
-        <v>2</v>
-      </c>
       <c r="T2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="12" t="s">
-        <v>2</v>
-      </c>
       <c r="W2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="Y2" s="9" t="s">
-        <v>2</v>
-      </c>
       <c r="Z2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="9" t="s">
-        <v>2</v>
-      </c>
       <c r="AC2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="9" t="s">
         <v>3</v>
+      </c>
+      <c r="AF2" s="10" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="10">
         <v>29000.0</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" s="10">
         <v>29000.0</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H3" s="10">
         <v>29000.0</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K3" s="10">
         <v>29000.0</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N3" s="10">
         <v>29000.0</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q3" s="10">
         <v>29000.0</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T3" s="10">
         <v>29000.0</v>
       </c>
       <c r="V3" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W3" s="10">
         <v>29000.0</v>
       </c>
       <c r="Y3" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Z3" s="13">
         <v>29000.0</v>
       </c>
       <c r="AB3" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC3" s="10">
         <v>29000.0</v>
       </c>
+      <c r="AE3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF3" s="10">
+        <v>29000.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="10">
         <v>16000.0</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" s="10">
         <v>16000.0</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H4" s="10">
         <v>16000.0</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K4" s="10">
         <v>16000.0</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N4" s="10">
         <v>16000.0</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q4" s="10">
         <v>16000.0</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T4" s="10">
         <v>16000.0</v>
       </c>
       <c r="V4" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W4" s="10">
         <v>16000.0</v>
       </c>
       <c r="Y4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Z4" s="13">
         <v>16000.0</v>
       </c>
       <c r="AB4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC4" s="10">
         <v>16000.0</v>
       </c>
+      <c r="AE4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF4" s="10">
+        <v>16000.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="K5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="N5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="Q5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="S5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="S5" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="T5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="V5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="V5" s="12" t="s">
-        <v>6</v>
-      </c>
       <c r="W5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="Y5" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="Z5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AB5" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="AC5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE5" s="9" t="s">
         <v>7</v>
+      </c>
+      <c r="AF5" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E6" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="K6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="N6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="P6" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="Q6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="S6" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="T6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="V6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="V6" s="12" t="s">
-        <v>8</v>
-      </c>
       <c r="W6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="Y6" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="Z6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AB6" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="AC6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE6" s="9" t="s">
         <v>9</v>
+      </c>
+      <c r="AF6" s="10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="14">
         <v>1.6241664E7</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="14">
         <v>1.6241664E7</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H7" s="14">
         <v>1.6241664E7</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K7" s="14">
         <v>1.6241664E7</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N7" s="14">
         <v>1.6241664E7</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q7" s="14">
         <v>1.6241664E7</v>
       </c>
       <c r="S7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T7" s="14">
         <v>1.6241664E7</v>
       </c>
       <c r="V7" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="W7" s="14">
         <v>1.6241664E7</v>
       </c>
       <c r="Y7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Z7" s="15">
         <v>1.6241664E7</v>
       </c>
       <c r="AB7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AC7" s="14">
         <v>1.6241664E7</v>
       </c>
+      <c r="AE7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF7" s="14">
+        <v>1.6241664E7</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="10">
         <v>0.25</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" s="10">
         <v>0.25</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H8" s="10">
         <v>5.0E-4</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K8" s="10">
         <v>0.001</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N8" s="10">
         <v>0.001</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q8" s="10">
         <v>0.001</v>
       </c>
       <c r="S8" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T8" s="10">
         <v>0.001</v>
       </c>
       <c r="V8" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="W8" s="10">
         <v>5.0E-4</v>
       </c>
       <c r="Y8" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Z8" s="13">
         <v>5.0E-4</v>
       </c>
       <c r="AB8" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AC8" s="10">
         <v>5.0E-4</v>
       </c>
+      <c r="AE8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF8" s="10">
+        <v>5.0E-4</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>12</v>
-      </c>
       <c r="E9" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="T9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="V9" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="W9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Y9" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Z9" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB9" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AC9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="AE9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF9" s="10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="10">
         <v>0.1</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" s="10">
         <v>0.1</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H10" s="10">
         <v>1.0</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K10" s="10">
         <v>1.0</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N10" s="10">
         <v>1.0</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q10" s="10">
         <v>1.0</v>
       </c>
       <c r="S10" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="T10" s="10">
         <v>1.0</v>
       </c>
       <c r="V10" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="W10" s="10">
         <v>1.0</v>
       </c>
       <c r="Y10" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Z10" s="13">
         <v>1.0</v>
       </c>
       <c r="AB10" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AC10" s="10">
         <v>1.0</v>
       </c>
+      <c r="AE10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF10" s="10">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="10"/>
       <c r="D11" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
       <c r="G11" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H11" s="10"/>
       <c r="J11" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M11" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="N11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="P11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q11" s="10" t="s">
+      <c r="S11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="S11" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="T11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="V11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="W11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF11" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="V11" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="W11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z11" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC11" s="10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="E12" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="K12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="N12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="P12" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="Q12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="S12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="S12" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="T12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="V12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="V12" s="12" t="s">
-        <v>22</v>
-      </c>
       <c r="W12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="Y12" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="Z12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AB12" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="AC12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE12" s="9" t="s">
         <v>23</v>
+      </c>
+      <c r="AF12" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="10">
         <v>1.0</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" s="10">
         <v>1.0</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H13" s="10">
         <v>1.0</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K13" s="10">
         <v>1.0</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N13" s="10">
         <v>2.0</v>
       </c>
       <c r="P13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q13" s="10">
         <v>1.0</v>
       </c>
       <c r="S13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T13" s="10">
         <v>2.0</v>
       </c>
       <c r="V13" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="W13" s="10">
         <v>1.0</v>
       </c>
       <c r="Y13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Z13" s="13">
         <v>2.0</v>
       </c>
       <c r="AB13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AC13" s="10">
         <v>2.0</v>
       </c>
+      <c r="AE13" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF13" s="10">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="10">
         <v>10.0</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E14" s="10">
         <v>10.0</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H14" s="10">
         <v>10.0</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K14" s="10">
         <v>10.0</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N14" s="10">
         <v>10.0</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q14" s="10">
         <v>10.0</v>
       </c>
       <c r="S14" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T14" s="10">
         <v>10.0</v>
       </c>
       <c r="V14" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W14" s="10">
         <v>10.0</v>
       </c>
       <c r="Y14" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Z14" s="13">
         <v>10.0</v>
       </c>
       <c r="AB14" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AC14" s="10">
         <v>10.0</v>
       </c>
+      <c r="AE14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF14" s="10">
+        <v>10.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" s="17">
         <v>126.2</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15" s="17">
         <v>144.1</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H15" s="17">
         <v>147.5</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K15" s="11">
         <v>129.1</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N15" s="11">
         <v>112.8</v>
       </c>
       <c r="P15" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q15" s="11">
         <v>129.1</v>
       </c>
       <c r="S15" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T15" s="11">
         <v>112.8</v>
       </c>
       <c r="V15" s="18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W15" s="11">
         <v>147.3</v>
       </c>
       <c r="X15" s="19"/>
       <c r="Y15" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Z15" s="20">
         <v>129.0</v>
       </c>
       <c r="AA15" s="21"/>
       <c r="AB15" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC15" s="11">
         <v>107.2</v>
       </c>
+      <c r="AE15" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF15" s="11">
+        <v>131.9</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="11">
         <f>B15/B14</f>
         <v>12.62</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E16" s="11">
         <f>E15/E14</f>
@@ -1628,49 +1737,49 @@
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H16" s="11">
         <f>H15/H14</f>
         <v>14.75</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K16" s="11">
         <f>K15/K14</f>
         <v>12.91</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N16" s="11">
         <f>N15/N14</f>
         <v>11.28</v>
       </c>
       <c r="P16" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q16" s="11">
         <f>Q15/Q14</f>
         <v>12.91</v>
       </c>
       <c r="S16" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T16" s="11">
         <f>T15/T14</f>
         <v>11.28</v>
       </c>
       <c r="V16" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W16" s="11">
         <f>W15/W14</f>
         <v>14.73</v>
       </c>
       <c r="Y16" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Z16" s="20">
         <f>Z15/Z14</f>
@@ -1681,7 +1790,7 @@
         <v>1.141860465</v>
       </c>
       <c r="AB16" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AC16" s="11">
         <f>AC15/AC14</f>
@@ -1691,633 +1800,685 @@
         <f>W16/AC16</f>
         <v>1.374067164</v>
       </c>
+      <c r="AE16" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF16" s="11">
+        <f>AF15/AF14</f>
+        <v>13.19</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="24"/>
       <c r="D17" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H17" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="J17" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="K17" s="23" t="s">
+      <c r="M17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="M17" s="22" t="s">
-        <v>28</v>
-      </c>
       <c r="N17" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="P17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="P17" s="22" t="s">
-        <v>28</v>
-      </c>
       <c r="Q17" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="S17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="S17" s="22" t="s">
-        <v>28</v>
-      </c>
       <c r="T17" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="U17" s="24"/>
       <c r="V17" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W17" s="23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Y17" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Z17" s="26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB17" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AC17" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE17" s="22" t="s">
         <v>29</v>
+      </c>
+      <c r="AF17" s="23" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="11">
         <v>1.0</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E18" s="11">
         <v>1.0</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H18" s="11">
         <v>1.0</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K18" s="11">
         <v>1.0</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N18" s="11">
         <v>1.0</v>
       </c>
       <c r="P18" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q18" s="11">
         <v>1.0</v>
       </c>
       <c r="S18" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T18" s="11">
         <v>1.0</v>
       </c>
       <c r="V18" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W18" s="11">
         <v>1.0</v>
       </c>
       <c r="Y18" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z18" s="20">
         <v>1.0</v>
       </c>
       <c r="AB18" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AC18" s="11">
         <v>1.0</v>
       </c>
+      <c r="AE18" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF18" s="11">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" s="11">
         <v>1140.0</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J19" s="16" t="s">
-        <v>33</v>
-      </c>
       <c r="K19" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M19" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="P19" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q19" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="S19" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="T19" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="V19" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="W19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="M19" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="N19" s="11" t="s">
+      <c r="Y19" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z19" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="P19" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q19" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="S19" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="T19" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="V19" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="W19" s="11" t="s">
+      <c r="AB19" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="Y19" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z19" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB19" s="16" t="s">
-        <v>33</v>
-      </c>
       <c r="AC19" s="11" t="s">
-        <v>36</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="AE19" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF19" s="11"/>
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B20" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="16" t="s">
-        <v>37</v>
-      </c>
       <c r="E20" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K20" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="N20" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="P20" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q20" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="S20" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="T20" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="V20" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="W20" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="M20" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="N20" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="P20" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q20" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="S20" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T20" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="V20" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="W20" s="11" t="s">
-        <v>40</v>
-      </c>
       <c r="Y20" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Z20" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AB20" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AC20" s="11"/>
+      <c r="AE20" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF20" s="11"/>
     </row>
     <row r="21">
       <c r="A21" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>44</v>
-      </c>
       <c r="E21" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K21" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="N21" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="P21" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q21" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="S21" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="T21" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="V21" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="W21" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="M21" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="N21" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="P21" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q21" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="S21" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="T21" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="V21" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="W21" s="11" t="s">
-        <v>47</v>
-      </c>
       <c r="Y21" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Z21" s="20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AB21" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AC21" s="11"/>
+      <c r="AE21" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF21" s="11"/>
     </row>
     <row r="22">
       <c r="A22" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="P22" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="S22" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="T22" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="V22" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="W22" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="M22" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="N22" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="P22" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q22" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="S22" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="T22" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="V22" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="W22" s="11" t="s">
-        <v>54</v>
-      </c>
       <c r="Y22" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Z22" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AB22" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AC22" s="11"/>
+      <c r="AE22" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF22" s="11"/>
     </row>
     <row r="23">
       <c r="A23" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M23" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="P23" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="S23" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="V23" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="W23" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="M23" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="N23" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="P23" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q23" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="S23" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="V23" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="W23" s="11" t="s">
-        <v>61</v>
-      </c>
       <c r="Y23" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z23" s="20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AB23" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AC23" s="11"/>
+      <c r="AE23" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF23" s="11"/>
     </row>
     <row r="24">
       <c r="A24" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K24" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M24" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="N24" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="P24" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q24" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="S24" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="T24" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="V24" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="W24" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="M24" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="N24" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="P24" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q24" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="S24" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="T24" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="V24" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="W24" s="11" t="s">
-        <v>68</v>
-      </c>
       <c r="Y24" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Z24" s="20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AB24" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AC24" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="AE24" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF24" s="11" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B25" s="11">
         <v>30.49523</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E25" s="11">
         <v>34.74433</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H25" s="11">
         <v>36.15689</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K25" s="11">
         <v>34.75708</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="N25" s="11">
         <v>35.72301</v>
       </c>
       <c r="P25" s="16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="Q25" s="11">
         <v>34.75708</v>
       </c>
       <c r="S25" s="16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="T25" s="11">
         <v>35.72301</v>
       </c>
       <c r="V25" s="18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="W25" s="11">
         <v>36.15689</v>
       </c>
       <c r="Y25" s="16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="Z25" s="20">
         <v>36.76593</v>
       </c>
       <c r="AB25" s="16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AC25" s="11">
         <v>35.07939</v>
       </c>
+      <c r="AE25" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF25" s="11"/>
     </row>
     <row r="26">
       <c r="A26" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E26" s="27">
         <v>33.1949</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H26" s="27">
         <v>34.82592</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K26" s="27">
         <v>33.61944</v>
       </c>
       <c r="M26" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N26" s="11">
         <v>34.0287</v>
       </c>
       <c r="P26" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q26" s="27">
         <v>33.61944</v>
       </c>
       <c r="S26" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="T26" s="11">
         <v>34.0287</v>
       </c>
       <c r="V26" s="28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="W26" s="29">
         <v>34.82592</v>
       </c>
       <c r="X26" s="30"/>
       <c r="Y26" s="31" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Z26" s="32">
         <v>35.31526</v>
       </c>
       <c r="AB26" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AC26" s="27">
         <v>32.74403</v>
+      </c>
+      <c r="AE26" s="16" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="28">
@@ -2331,156 +2492,439 @@
       <c r="C29" s="2"/>
       <c r="E29" s="33"/>
       <c r="F29" s="2"/>
+      <c r="AB29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE29" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="30">
       <c r="B30" s="33"/>
       <c r="C30" s="2"/>
       <c r="E30" s="33"/>
       <c r="F30" s="2"/>
+      <c r="AB30" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE30" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF30" s="10" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" s="33"/>
       <c r="C31" s="2"/>
       <c r="E31" s="33"/>
       <c r="F31" s="2"/>
+      <c r="AB31" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC31" s="10">
+        <v>29000.0</v>
+      </c>
+      <c r="AE31" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF31" s="10">
+        <v>29000.0</v>
+      </c>
     </row>
     <row r="32">
       <c r="B32" s="33"/>
       <c r="C32" s="2"/>
       <c r="E32" s="33"/>
       <c r="F32" s="2"/>
+      <c r="AB32" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC32" s="10">
+        <v>16000.0</v>
+      </c>
+      <c r="AE32" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF32" s="10">
+        <v>16000.0</v>
+      </c>
     </row>
     <row r="33">
       <c r="B33" s="33"/>
       <c r="C33" s="2"/>
       <c r="E33" s="33"/>
       <c r="F33" s="2"/>
+      <c r="AB33" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC33" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE33" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF33" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" s="33"/>
       <c r="C34" s="2"/>
       <c r="E34" s="33"/>
       <c r="F34" s="2"/>
+      <c r="AB34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC34" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF34" s="10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="35">
       <c r="B35" s="33"/>
       <c r="C35" s="2"/>
       <c r="E35" s="33"/>
       <c r="F35" s="2"/>
+      <c r="AB35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC35" s="14">
+        <v>1.6241664E7</v>
+      </c>
+      <c r="AE35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF35" s="14">
+        <v>1.6241664E7</v>
+      </c>
     </row>
     <row r="36">
       <c r="B36" s="33"/>
       <c r="C36" s="2"/>
       <c r="E36" s="33"/>
       <c r="F36" s="2"/>
+      <c r="AB36" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC36" s="10">
+        <v>5.0E-4</v>
+      </c>
+      <c r="AE36" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF36" s="10">
+        <v>5.0E-4</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="33"/>
       <c r="C37" s="2"/>
       <c r="E37" s="33"/>
       <c r="F37" s="2"/>
+      <c r="AB37" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC37" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE37" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF37" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="38">
       <c r="B38" s="33"/>
       <c r="C38" s="2"/>
       <c r="E38" s="33"/>
       <c r="F38" s="2"/>
+      <c r="AB38" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC38" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="AE38" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF38" s="10">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="39">
       <c r="B39" s="33"/>
       <c r="C39" s="2"/>
       <c r="E39" s="33"/>
       <c r="F39" s="2"/>
+      <c r="AB39" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC39" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE39" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF39" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="40">
       <c r="B40" s="33"/>
       <c r="C40" s="2"/>
       <c r="E40" s="33"/>
       <c r="F40" s="2"/>
+      <c r="AB40" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC40" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE40" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF40" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="41">
       <c r="B41" s="33"/>
       <c r="C41" s="2"/>
       <c r="E41" s="33"/>
       <c r="F41" s="2"/>
+      <c r="AB41" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC41" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="AE41" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF41" s="10">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="42">
       <c r="B42" s="33"/>
       <c r="C42" s="2"/>
       <c r="E42" s="33"/>
       <c r="F42" s="2"/>
+      <c r="AB42" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC42" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="AE42" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF42" s="10">
+        <v>10.0</v>
+      </c>
     </row>
     <row r="43">
       <c r="B43" s="33"/>
       <c r="C43" s="2"/>
       <c r="E43" s="33"/>
       <c r="F43" s="2"/>
+      <c r="AB43" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC43" s="11">
+        <v>103.3</v>
+      </c>
+      <c r="AE43" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF43" s="11">
+        <v>120.2</v>
+      </c>
     </row>
     <row r="44">
       <c r="B44" s="33"/>
       <c r="C44" s="2"/>
       <c r="E44" s="33"/>
       <c r="F44" s="2"/>
+      <c r="AB44" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC44" s="11">
+        <f>AC43/AC42</f>
+        <v>10.33</v>
+      </c>
+      <c r="AD44" s="21"/>
+      <c r="AE44" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF44" s="11">
+        <f>AF43/AF42</f>
+        <v>12.02</v>
+      </c>
     </row>
     <row r="45">
       <c r="B45" s="33"/>
       <c r="C45" s="2"/>
       <c r="E45" s="33"/>
       <c r="F45" s="2"/>
+      <c r="AB45" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC45" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE45" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF45" s="23" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="46">
       <c r="B46" s="33"/>
       <c r="C46" s="2"/>
       <c r="E46" s="33"/>
       <c r="F46" s="2"/>
+      <c r="AB46" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC46" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="AE46" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF46" s="11">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="47">
       <c r="B47" s="33"/>
       <c r="C47" s="2"/>
       <c r="E47" s="33"/>
       <c r="F47" s="2"/>
+      <c r="AB47" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC47" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE47" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF47" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="48">
       <c r="B48" s="33"/>
       <c r="C48" s="2"/>
       <c r="E48" s="33"/>
       <c r="F48" s="2"/>
+      <c r="AB48" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC48" s="11"/>
+      <c r="AE48" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF48" s="11"/>
     </row>
     <row r="49">
       <c r="B49" s="33"/>
       <c r="C49" s="2"/>
       <c r="E49" s="33"/>
       <c r="F49" s="2"/>
+      <c r="AB49" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC49" s="11"/>
+      <c r="AE49" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF49" s="11"/>
     </row>
     <row r="50">
       <c r="B50" s="33"/>
       <c r="C50" s="2"/>
       <c r="E50" s="33"/>
       <c r="F50" s="2"/>
+      <c r="AB50" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC50" s="11"/>
+      <c r="AE50" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF50" s="11"/>
     </row>
     <row r="51">
       <c r="B51" s="33"/>
       <c r="C51" s="2"/>
       <c r="E51" s="33"/>
       <c r="F51" s="2"/>
+      <c r="AB51" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC51" s="11"/>
+      <c r="AE51" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF51" s="11"/>
     </row>
     <row r="52">
       <c r="B52" s="33"/>
       <c r="C52" s="2"/>
       <c r="E52" s="33"/>
       <c r="F52" s="2"/>
+      <c r="AB52" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC52" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE52" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF52" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="53">
       <c r="B53" s="33"/>
       <c r="C53" s="2"/>
       <c r="E53" s="33"/>
       <c r="F53" s="2"/>
+      <c r="AB53" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC53" s="11"/>
+      <c r="AE53" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF53" s="11"/>
     </row>
     <row r="54">
       <c r="B54" s="33"/>
       <c r="C54" s="2"/>
       <c r="E54" s="33"/>
       <c r="F54" s="2"/>
+      <c r="AB54" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE54" s="16" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="55">
       <c r="B55" s="33"/>
@@ -8219,7 +8663,7 @@
       <c r="F1010" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="13">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
@@ -8230,6 +8674,9 @@
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AB29:AC29"/>
+    <mergeCell ref="AE29:AF29"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -8259,36 +8706,36 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>2</v>
-      </c>
       <c r="E2" s="10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="10"/>
     </row>
     <row r="3">
       <c r="A3" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="10">
         <v>29000.0</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" s="10">
         <v>29000.0</v>
@@ -8298,61 +8745,61 @@
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="10">
         <v>16000.0</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="10"/>
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="E5" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="10"/>
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E6" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="10"/>
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="14">
         <v>1.6241664E7</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="14">
         <v>9038341.0</v>
@@ -8362,13 +8809,13 @@
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="10">
         <v>5.0E-4</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" s="10">
         <v>5.0E-4</v>
@@ -8378,29 +8825,29 @@
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="10"/>
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="10">
         <v>1.0</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" s="10">
         <v>1.0</v>
@@ -8410,45 +8857,45 @@
     </row>
     <row r="11">
       <c r="A11" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="10"/>
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="E12" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="10"/>
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="10">
         <v>1.0</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" s="10">
         <v>1.0</v>
@@ -8458,13 +8905,13 @@
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="10">
         <v>10.0</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E14" s="10">
         <v>10.0</v>
@@ -8474,7 +8921,7 @@
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" s="11">
         <v>147.3</v>
@@ -8484,7 +8931,7 @@
         <v>1.133076923</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15" s="17">
         <v>130.0</v>
@@ -8498,14 +8945,14 @@
     </row>
     <row r="16">
       <c r="A16" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="11">
         <f>B15/B14</f>
         <v>14.73</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E16" s="11">
         <v>13.0</v>
@@ -8515,13 +8962,13 @@
     </row>
     <row r="17">
       <c r="A17" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E17" s="23">
         <v>128.0</v>
@@ -8531,13 +8978,13 @@
     </row>
     <row r="18">
       <c r="A18" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="11">
         <v>1.0</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E18" s="11">
         <v>1.0</v>
@@ -8547,29 +8994,29 @@
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="16" t="s">
-        <v>33</v>
-      </c>
       <c r="E19" s="11" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="11"/>
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E20" s="11">
         <v>0.976</v>
@@ -8579,13 +9026,13 @@
     </row>
     <row r="21">
       <c r="A21" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E21" s="11">
         <v>2.653</v>
@@ -8595,13 +9042,13 @@
     </row>
     <row r="22">
       <c r="A22" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E22" s="11">
         <v>1.635</v>
@@ -8611,13 +9058,13 @@
     </row>
     <row r="23">
       <c r="A23" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E23" s="11">
         <v>5.127</v>
@@ -8627,45 +9074,45 @@
     </row>
     <row r="24">
       <c r="A24" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="11"/>
     </row>
     <row r="25">
       <c r="A25" s="16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B25" s="11">
         <v>36.15689</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="11"/>
     </row>
     <row r="26">
       <c r="A26" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B26" s="27">
         <v>34.82592</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E26" s="11">
         <v>35.74</v>

</xml_diff>